<commit_message>
added tab for printing
</commit_message>
<xml_diff>
--- a/correlations_summary.xlsx
+++ b/correlations_summary.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18250" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18250" windowHeight="7530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="correlations" sheetId="1" r:id="rId1"/>
+    <sheet name="To print" sheetId="3" r:id="rId2"/>
+    <sheet name="all data" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="27">
   <si>
     <t>Answer.duration</t>
   </si>
@@ -57,12 +59,115 @@
   <si>
     <t>p-values</t>
   </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <r>
+      <t>High degree:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> If the coefficient value lies between ± 0.50 and ± 1, then it is said to be a strong correlation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Moderate degree:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> If the value lies between ± 0.30 and ± 0.49, then it is said to be a medium correlation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Low degree:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> When the value lies below </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t> .29, then it is said to be a small correlation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>No correlation: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>When the value is zero.</t>
+    </r>
+  </si>
+  <si>
+    <t>Answer duration</t>
+  </si>
+  <si>
+    <t>Answer confidence</t>
+  </si>
+  <si>
+    <t>Answer difficulty</t>
+  </si>
+  <si>
+    <t>Worker age</t>
+  </si>
+  <si>
+    <t>Worker score</t>
+  </si>
+  <si>
+    <t>Code LOC</t>
+  </si>
+  <si>
+    <t>Code complexity</t>
+  </si>
+  <si>
+    <t>Answer explanation size</t>
+  </si>
+  <si>
+    <t>Worker years of experience</t>
+  </si>
+  <si>
+    <t>Code 
+LOC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,8 +302,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,8 +519,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -543,6 +690,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -588,7 +889,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -615,6 +916,93 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="37" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="37" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="37" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -662,38 +1050,416 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
+  <dxfs count="101">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -718,8 +1484,488 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9B9B"/>
+      <color rgb="FFFF8181"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -732,19 +1978,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:J11" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A2:J11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:J11" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
   <tableColumns count="10">
-    <tableColumn id="1" name="Spearman Correlations" dataDxfId="11"/>
-    <tableColumn id="2" name="Answer.duration" dataDxfId="10"/>
-    <tableColumn id="3" name="Answer.confidence" dataDxfId="9"/>
-    <tableColumn id="4" name="Answer.difficulty" dataDxfId="8"/>
-    <tableColumn id="5" name="Answer.explanationSize" dataDxfId="7"/>
-    <tableColumn id="6" name="Worker.age" dataDxfId="6"/>
-    <tableColumn id="7" name="Worker.score" dataDxfId="5"/>
-    <tableColumn id="8" name="Worker.yearsOfExperience" dataDxfId="4"/>
-    <tableColumn id="9" name="Code.LOC" dataDxfId="3"/>
-    <tableColumn id="10" name="Code.complexity" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Spearman Correlations" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Answer duration" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Answer confidence" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Answer difficulty" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Answer explanation size" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Worker age" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Worker score" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Worker years of experience" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Code LOC" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Code complexity" dataDxfId="46"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4B5F11E4-5E24-4054-B6D4-ED3B94FABD18}" name="Table24" displayName="Table24" ref="B2:K11" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{4F714E52-3F99-4F56-BD89-6FA1188743F2}" name="Spearman Correlations" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{E0D31532-DE9E-44D8-9799-C022B6443DE7}" name="Answer duration" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{1A3147C9-3BD6-4F3B-9592-1C5186DB9244}" name="Answer confidence" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{FEA07AB3-00F6-4E31-A141-3F226F485D5B}" name="Answer difficulty" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{ED1BFFE6-EE12-4E65-A76F-C784F3447516}" name="Answer explanation size" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{F2D8C1B7-CF67-4E1B-A8E6-D8C4967A4554}" name="Worker age" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{95A941AA-5DB2-41A5-A857-5E2FC76D8B2A}" name="Worker years of experience" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{C630A903-D1E6-4D97-9CFC-DB37A1FA5320}" name="Worker score" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{9A171F83-996D-47A0-9F45-1E955DCAB90A}" name="Code _x000a_LOC" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{606C51F5-12AD-492C-97A0-2D59C0F93C37}" name="Code complexity" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F69AC107-BB49-4113-99A4-580D7C96FAD4}" name="Table22" displayName="Table22" ref="A2:J11" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
+  <autoFilter ref="A2:J11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{730CCBB1-AC15-4F76-8658-499BBF9F327F}" name="Spearman Correlations" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{2EF649F7-CBCF-4119-8704-8609DC0A4191}" name="Answer.duration" dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{BE79A77D-6E82-40E7-8879-451657BD2470}" name="Answer.confidence" dataDxfId="94"/>
+    <tableColumn id="4" xr3:uid="{21C02CF1-E6F8-4239-BC96-BE39B764CBEA}" name="Answer.difficulty" dataDxfId="93"/>
+    <tableColumn id="5" xr3:uid="{C4282863-51A2-429F-A3BC-50D41BBC3125}" name="Answer.explanationSize" dataDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{9256A6DC-68D4-4917-8E93-83FCBD5504DC}" name="Worker.age" dataDxfId="91"/>
+    <tableColumn id="7" xr3:uid="{B5CC5391-D9E0-49B0-95E4-731CDFC8B119}" name="Worker.score" dataDxfId="90"/>
+    <tableColumn id="8" xr3:uid="{F1CEFE01-8A25-4892-8EFF-12BBA59C483B}" name="Worker.yearsOfExperience" dataDxfId="89"/>
+    <tableColumn id="9" xr3:uid="{E0A74493-B88F-40E5-BEC9-8F4B93285734}" name="Code.LOC" dataDxfId="88"/>
+    <tableColumn id="10" xr3:uid="{96BB921C-6A27-4AA9-98A7-349D678C9C71}" name="Code.complexity" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1046,14 +2328,1115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:J29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.1796875" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="24.08984375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.90625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="18.1796875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" ht="29">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
+        <v>-9.3390814960002899E-2</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.12364736199379001</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0.45176514983177202</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.17628009617328599</v>
+      </c>
+      <c r="G3" s="11">
+        <v>6.9619752466678606E-2</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0.145769342780113</v>
+      </c>
+      <c r="I3" s="11">
+        <v>7.1861594915390001E-2</v>
+      </c>
+      <c r="J3" s="11">
+        <v>7.1861594915390001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="11">
+        <v>-9.3390814960002899E-2</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11">
+        <v>-0.57210046052932695</v>
+      </c>
+      <c r="E4" s="11">
+        <v>9.1033250093460097E-2</v>
+      </c>
+      <c r="F4" s="11">
+        <v>4.8283178359270103E-2</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.221997395157814</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0.12364736199379001</v>
+      </c>
+      <c r="C5" s="11">
+        <v>-0.57210046052932695</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11">
+        <v>-0.126304566860199</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="11">
+        <v>-8.5856214165687603E-2</v>
+      </c>
+      <c r="H5" s="11">
+        <v>-0.24901738762855499</v>
+      </c>
+      <c r="I5" s="11">
+        <v>6.8165458738803905E-2</v>
+      </c>
+      <c r="J5" s="11">
+        <v>3.8963541388511699E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0.45176514983177202</v>
+      </c>
+      <c r="C6" s="11">
+        <v>9.1033250093460097E-2</v>
+      </c>
+      <c r="D6" s="11">
+        <v>-0.126304566860199</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.112209625542164</v>
+      </c>
+      <c r="G6" s="11">
+        <v>7.8005611896514906E-2</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0.22810959815979001</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="11">
+        <v>4.1282296180725098E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.17628009617328599</v>
+      </c>
+      <c r="C7" s="11">
+        <v>4.8283178359270103E-2</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.112209625542164</v>
+      </c>
+      <c r="F7" s="12">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11">
+        <v>5.1044616848230397E-2</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.55862081050872803</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="11">
+        <v>6.9619752466678606E-2</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="11">
+        <v>-8.5856214165687603E-2</v>
+      </c>
+      <c r="E8" s="11">
+        <v>7.8005611896514906E-2</v>
+      </c>
+      <c r="F8" s="11">
+        <v>5.1044616848230397E-2</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0.12306752055883401</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="11">
+        <v>-4.0266912430524798E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0.145769342780113</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.221997395157814</v>
+      </c>
+      <c r="D9" s="11">
+        <v>-0.24901738762855499</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.22810959815979001</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.55862081050872803</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0.12306752055883401</v>
+      </c>
+      <c r="H9" s="12">
+        <v>1</v>
+      </c>
+      <c r="I9" s="11">
+        <v>-4.7836016863584498E-2</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="11">
+        <v>7.1861594915390001E-2</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="11">
+        <v>6.8165458738803905E-2</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="11">
+        <v>-4.7836016863584498E-2</v>
+      </c>
+      <c r="I10" s="12">
+        <v>1</v>
+      </c>
+      <c r="J10" s="11">
+        <v>0.63391876220703103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="11">
+        <v>7.5235642492771093E-2</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="11">
+        <v>3.8963541388511699E-2</v>
+      </c>
+      <c r="E11" s="11">
+        <v>4.1282296180725098E-2</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="11">
+        <v>-4.0266912430524798E-2</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0.63391876220703103</v>
+      </c>
+      <c r="J11" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2.23961172096665E-6</v>
+      </c>
+      <c r="D15" s="6">
+        <v>3.5306735313156403E-10</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>4.2668980684945602E-4</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1.2922996006636799E-13</v>
+      </c>
+      <c r="I15" s="6">
+        <v>2.7611514861813902E-4</v>
+      </c>
+      <c r="J15" s="6">
+        <v>1.4011664505009201E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8">
+        <v>2.23961172096665E-6</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
+        <v>4.0153987557189899E-6</v>
+      </c>
+      <c r="F16" s="8">
+        <v>1.46160412084604E-2</v>
+      </c>
+      <c r="G16" s="8">
+        <v>5.3358099624826003E-2</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0</v>
+      </c>
+      <c r="I16" s="8">
+        <v>5.3194435608916499E-2</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0.23477756000501701</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="6">
+        <v>3.5306735313156403E-10</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1.4611645227091701E-10</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0.31795557096689597</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1.37773958956977E-5</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0</v>
+      </c>
+      <c r="I17" s="6">
+        <v>5.6217686439330396E-4</v>
+      </c>
+      <c r="J17" s="6">
+        <v>4.88331220954994E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="8">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8">
+        <v>4.0153987557189899E-6</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1.4611645227091701E-10</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1.27575308095373E-8</v>
+      </c>
+      <c r="G18" s="8">
+        <v>7.86154756267088E-5</v>
+      </c>
+      <c r="H18" s="8">
+        <v>0</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0.92500884385868098</v>
+      </c>
+      <c r="J18" s="8">
+        <v>3.6853600081859998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1.46160412084604E-2</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.31795557096689597</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1.27575308095373E-8</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="6">
+        <v>9.8348297600794297E-3</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.110005151050098</v>
+      </c>
+      <c r="J19" s="6">
+        <v>0.15685758867456601</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="8">
+        <v>4.2668980684945602E-4</v>
+      </c>
+      <c r="C20" s="8">
+        <v>5.3358099624826003E-2</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1.37773958956977E-5</v>
+      </c>
+      <c r="E20" s="8">
+        <v>7.86154756267088E-5</v>
+      </c>
+      <c r="F20" s="8">
+        <v>9.8348297600794297E-3</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="8">
+        <v>4.2697312352402202E-10</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0.571172639781235</v>
+      </c>
+      <c r="J20" s="8">
+        <v>4.1750504530216198E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1.2922996006636799E-13</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <v>4.2697312352402202E-10</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="6">
+        <v>1.55582857884866E-2</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0.96107509958246196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="8">
+        <v>2.7611514861813902E-4</v>
+      </c>
+      <c r="C22" s="8">
+        <v>5.3194435608916499E-2</v>
+      </c>
+      <c r="D22" s="8">
+        <v>5.6217686439330396E-4</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0.92500884385868098</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0.110005151050098</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.571172639781235</v>
+      </c>
+      <c r="H22" s="8">
+        <v>1.55582857884866E-2</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="6">
+        <v>1.4011664505009201E-4</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.23477756000501701</v>
+      </c>
+      <c r="D23" s="6">
+        <v>4.88331220954994E-2</v>
+      </c>
+      <c r="E23" s="6">
+        <v>3.6853600081859998E-2</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.15685758867456601</v>
+      </c>
+      <c r="G23" s="6">
+        <v>4.1750504530216198E-2</v>
+      </c>
+      <c r="H23" s="6">
+        <v>0.96107509958246196</v>
+      </c>
+      <c r="I23" s="6">
+        <v>0</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="D26" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="D27" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="D28" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="D29" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B15:I23">
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:J23">
+    <cfRule type="cellIs" dxfId="28" priority="7" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:J11">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="between">
+      <formula>-0.29</formula>
+      <formula>-0.001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="between">
+      <formula>0.001</formula>
+      <formula>0.29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="between">
+      <formula>-0.49</formula>
+      <formula>-0.3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="between">
+      <formula>0.3</formula>
+      <formula>0.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="between">
+      <formula>-1</formula>
+      <formula>-0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="between">
+      <formula>0.5</formula>
+      <formula>0.9999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932A3AE4-BA18-48EB-8066-24A92C3920A7}">
+  <dimension ref="B1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="24.08984375" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="15" thickBot="1"/>
+    <row r="2" spans="2:11" ht="44" thickBot="1">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="19">
+        <v>1</v>
+      </c>
+      <c r="D3" s="20">
+        <v>-9.3390814960002899E-2</v>
+      </c>
+      <c r="E3" s="20">
+        <v>0.12364736199379001</v>
+      </c>
+      <c r="F3" s="21">
+        <v>0.45176514983177202</v>
+      </c>
+      <c r="G3" s="33">
+        <v>0.17628009617328599</v>
+      </c>
+      <c r="H3" s="24">
+        <v>0.145769342780113</v>
+      </c>
+      <c r="I3" s="24">
+        <v>6.9619752466678606E-2</v>
+      </c>
+      <c r="J3" s="33">
+        <v>7.1861594915390001E-2</v>
+      </c>
+      <c r="K3" s="25">
+        <v>7.1861594915390001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="22">
+        <v>-9.3390814960002899E-2</v>
+      </c>
+      <c r="D4" s="23">
+        <v>1</v>
+      </c>
+      <c r="E4" s="24">
+        <v>-0.57210046052932695</v>
+      </c>
+      <c r="F4" s="25">
+        <v>9.1033250093460097E-2</v>
+      </c>
+      <c r="G4" s="33">
+        <v>4.8283178359270103E-2</v>
+      </c>
+      <c r="H4" s="24">
+        <v>0.221997395157814</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="22">
+        <v>0.12364736199379001</v>
+      </c>
+      <c r="D5" s="26">
+        <v>-0.57210046052932695</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1</v>
+      </c>
+      <c r="F5" s="25">
+        <v>-0.126304566860199</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="24">
+        <v>-0.24901738762855499</v>
+      </c>
+      <c r="I5" s="24">
+        <v>-8.5856214165687603E-2</v>
+      </c>
+      <c r="J5" s="33">
+        <v>6.8165458738803905E-2</v>
+      </c>
+      <c r="K5" s="25">
+        <v>3.8963541388511699E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="15" thickBot="1">
+      <c r="B6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="27">
+        <v>0.45176514983177202</v>
+      </c>
+      <c r="D6" s="28">
+        <v>9.1033250093460097E-2</v>
+      </c>
+      <c r="E6" s="28">
+        <v>-0.126304566860199</v>
+      </c>
+      <c r="F6" s="29">
+        <v>1</v>
+      </c>
+      <c r="G6" s="33">
+        <v>0.112209625542164</v>
+      </c>
+      <c r="H6" s="24">
+        <v>0.22810959815979001</v>
+      </c>
+      <c r="I6" s="24">
+        <v>7.8005611896514906E-2</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="25">
+        <v>4.1282296180725098E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="34">
+        <v>0.17628009617328599</v>
+      </c>
+      <c r="D7" s="35">
+        <v>4.8283178359270103E-2</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="35">
+        <v>0.112209625542164</v>
+      </c>
+      <c r="G7" s="19">
+        <v>1</v>
+      </c>
+      <c r="H7" s="20">
+        <v>0.55862081050872803</v>
+      </c>
+      <c r="I7" s="20">
+        <v>5.1044616848230397E-2</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="22">
+        <v>0.145769342780113</v>
+      </c>
+      <c r="D8" s="26">
+        <v>0.221997395157814</v>
+      </c>
+      <c r="E8" s="26">
+        <v>-0.24901738762855499</v>
+      </c>
+      <c r="F8" s="26">
+        <v>0.22810959815979001</v>
+      </c>
+      <c r="G8" s="22">
+        <v>0.55862081050872803</v>
+      </c>
+      <c r="H8" s="23">
+        <v>1</v>
+      </c>
+      <c r="I8" s="24">
+        <v>0.12306752055883401</v>
+      </c>
+      <c r="J8" s="33">
+        <v>-4.7836016863584498E-2</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="15" thickBot="1">
+      <c r="B9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="22">
+        <v>6.9619752466678606E-2</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="26">
+        <v>-8.5856214165687603E-2</v>
+      </c>
+      <c r="F9" s="26">
+        <v>7.8005611896514906E-2</v>
+      </c>
+      <c r="G9" s="22">
+        <v>5.1044616848230397E-2</v>
+      </c>
+      <c r="H9" s="26">
+        <v>0.12306752055883401</v>
+      </c>
+      <c r="I9" s="23">
+        <v>1</v>
+      </c>
+      <c r="J9" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="25">
+        <v>-4.0266912430524798E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="35">
+        <v>7.1861594915390001E-2</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="35">
+        <v>6.8165458738803905E-2</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="35">
+        <v>-4.7836016863584498E-2</v>
+      </c>
+      <c r="I10" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="19">
+        <v>1</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0.63391876220703103</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="15" thickBot="1">
+      <c r="B11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="28">
+        <v>7.5235642492771093E-2</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="28">
+        <v>3.8963541388511699E-2</v>
+      </c>
+      <c r="F11" s="28">
+        <v>4.1282296180725098E-2</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="28">
+        <v>-4.0266912430524798E-2</v>
+      </c>
+      <c r="J11" s="27">
+        <v>0.63391876220703103</v>
+      </c>
+      <c r="K11" s="29">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C3 C6:F6 C5:E5 C4:D4 I9 J11:K11 J10 C10:I11 C8:H9 C7:G7">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="between">
+      <formula>-0.29</formula>
+      <formula>-0.001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="between">
+      <formula>0.001</formula>
+      <formula>0.29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="between">
+      <formula>-0.49</formula>
+      <formula>-0.3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="between">
+      <formula>0.3</formula>
+      <formula>0.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="between">
+      <formula>-1</formula>
+      <formula>-0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="between">
+      <formula>0.5</formula>
+      <formula>0.9999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4057CCF5-1814-44E2-B1C5-EC97704B62C3}">
   <dimension ref="A2:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="18.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="18.1796875" style="3"/>
     <col min="2" max="2" width="16.453125" style="3" customWidth="1"/>
@@ -1061,7 +3444,7 @@
     <col min="5" max="16384" width="18.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="29">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1093,7 +3476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +3508,7 @@
         <v>7.5235642492771093E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1157,7 +3540,7 @@
         <v>-2.3504732176661498E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1189,7 +3572,7 @@
         <v>3.8963541388511699E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1221,7 +3604,7 @@
         <v>4.1282296180725098E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1253,7 +3636,7 @@
         <v>2.8005229309201199E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1285,7 +3668,7 @@
         <v>-4.0266912430524798E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1317,7 +3700,7 @@
         <v>9.6562114777043505E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1349,7 +3732,7 @@
         <v>0.63391876220703103</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1381,7 +3764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -1413,7 +3796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
@@ -1445,7 +3828,7 @@
         <v>1.4011664505009201E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
         <v>1</v>
       </c>
@@ -1477,7 +3860,7 @@
         <v>0.23477756000501701</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10">
       <c r="A17" s="5" t="s">
         <v>2</v>
       </c>
@@ -1509,7 +3892,7 @@
         <v>4.88331220954994E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10">
       <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
@@ -1541,7 +3924,7 @@
         <v>3.6853600081859998E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10">
       <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
@@ -1573,7 +3956,7 @@
         <v>0.15685758867456601</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10">
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
@@ -1605,7 +3988,7 @@
         <v>4.1750504530216198E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10">
       <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
@@ -1637,7 +4020,7 @@
         <v>0.96107509958246196</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10">
       <c r="A22" s="5" t="s">
         <v>7</v>
       </c>
@@ -1669,7 +4052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10">
       <c r="A23" s="5" t="s">
         <v>8</v>
       </c>
@@ -1702,9 +4085,20 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="expression" dxfId="15" priority="2">
+      <formula>$B$15&lt;0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:I23">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added worker profession and correl with accuracy
</commit_message>
<xml_diff>
--- a/correlations_summary.xlsx
+++ b/correlations_summary.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18250" windowHeight="7530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18250" windowHeight="7530" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="correlations" sheetId="1" r:id="rId1"/>
     <sheet name="To print" sheetId="3" r:id="rId2"/>
     <sheet name="all data" sheetId="2" r:id="rId3"/>
+    <sheet name="accuracy" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="33">
   <si>
     <t>Answer.duration</t>
   </si>
@@ -162,12 +163,30 @@
     <t>Code 
 LOC</t>
   </si>
+  <si>
+    <t>Kendall  tau correlations</t>
+  </si>
+  <si>
+    <t>Answer accuracy</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Worker profession</t>
+  </si>
+  <si>
+    <t>Worker.profession</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,8 +345,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -537,8 +563,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -752,19 +790,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -839,6 +864,96 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -889,7 +1004,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -942,67 +1057,169 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="37" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="37" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="36" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="37" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="37" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="37" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="36" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="21" fillId="37" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="21" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="38" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="39" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="35" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="35" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="39" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1050,7 +1267,565 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="101">
+  <dxfs count="103">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1104,211 +1879,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9B9B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9B9B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9B9B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9B9B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1325,48 +1895,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9B9B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1654,302 +2182,6 @@
           <bgColor theme="1" tint="0.499984740745262"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9B9B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9B9B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9B9B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9B9B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9B9B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1978,55 +2210,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:J11" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Spearman Correlations" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Answer duration" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Answer confidence" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Answer difficulty" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Answer explanation size" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Worker age" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Worker score" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Worker years of experience" dataDxfId="48"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Code LOC" dataDxfId="47"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Code complexity" dataDxfId="46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:K12" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Spearman Correlations" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Answer duration" dataDxfId="99"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Answer confidence" dataDxfId="98"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Answer difficulty" dataDxfId="97"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Answer explanation size" dataDxfId="96"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Worker age" dataDxfId="95"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Worker score" dataDxfId="94"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Worker years of experience" dataDxfId="93"/>
+    <tableColumn id="11" xr3:uid="{C85195FD-52B3-4456-9A9D-7D225411B828}" name="Worker profession" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Code LOC" dataDxfId="92"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Code complexity" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4B5F11E4-5E24-4054-B6D4-ED3B94FABD18}" name="Table24" displayName="Table24" ref="B2:K11" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4F714E52-3F99-4F56-BD89-6FA1188743F2}" name="Spearman Correlations" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{E0D31532-DE9E-44D8-9799-C022B6443DE7}" name="Answer duration" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{1A3147C9-3BD6-4F3B-9592-1C5186DB9244}" name="Answer confidence" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{FEA07AB3-00F6-4E31-A141-3F226F485D5B}" name="Answer difficulty" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{ED1BFFE6-EE12-4E65-A76F-C784F3447516}" name="Answer explanation size" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{F2D8C1B7-CF67-4E1B-A8E6-D8C4967A4554}" name="Worker age" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{95A941AA-5DB2-41A5-A857-5E2FC76D8B2A}" name="Worker years of experience" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{C630A903-D1E6-4D97-9CFC-DB37A1FA5320}" name="Worker score" dataDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{9A171F83-996D-47A0-9F45-1E955DCAB90A}" name="Code _x000a_LOC" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{606C51F5-12AD-492C-97A0-2D59C0F93C37}" name="Code complexity" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4B5F11E4-5E24-4054-B6D4-ED3B94FABD18}" name="Table24" displayName="Table24" ref="B2:L12" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{4F714E52-3F99-4F56-BD89-6FA1188743F2}" name="Spearman Correlations" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{E0D31532-DE9E-44D8-9799-C022B6443DE7}" name="Answer duration" dataDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{1A3147C9-3BD6-4F3B-9592-1C5186DB9244}" name="Answer confidence" dataDxfId="86"/>
+    <tableColumn id="4" xr3:uid="{FEA07AB3-00F6-4E31-A141-3F226F485D5B}" name="Answer difficulty" dataDxfId="85"/>
+    <tableColumn id="5" xr3:uid="{ED1BFFE6-EE12-4E65-A76F-C784F3447516}" name="Answer explanation size" dataDxfId="84"/>
+    <tableColumn id="6" xr3:uid="{F2D8C1B7-CF67-4E1B-A8E6-D8C4967A4554}" name="Worker age" dataDxfId="83"/>
+    <tableColumn id="8" xr3:uid="{95A941AA-5DB2-41A5-A857-5E2FC76D8B2A}" name="Worker years of experience" dataDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{C630A903-D1E6-4D97-9CFC-DB37A1FA5320}" name="Worker score" dataDxfId="81"/>
+    <tableColumn id="11" xr3:uid="{0E4F1937-D49D-4AB2-9F32-8DDDF4A6B54B}" name="Worker profession"/>
+    <tableColumn id="9" xr3:uid="{9A171F83-996D-47A0-9F45-1E955DCAB90A}" name="Code _x000a_LOC" dataDxfId="80"/>
+    <tableColumn id="10" xr3:uid="{606C51F5-12AD-492C-97A0-2D59C0F93C37}" name="Code complexity" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F69AC107-BB49-4113-99A4-580D7C96FAD4}" name="Table22" displayName="Table22" ref="A2:J11" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F69AC107-BB49-4113-99A4-580D7C96FAD4}" name="Table22" displayName="Table22" ref="A2:J11" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <autoFilter ref="A2:J11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{730CCBB1-AC15-4F76-8658-499BBF9F327F}" name="Spearman Correlations" dataDxfId="96"/>
-    <tableColumn id="2" xr3:uid="{2EF649F7-CBCF-4119-8704-8609DC0A4191}" name="Answer.duration" dataDxfId="95"/>
-    <tableColumn id="3" xr3:uid="{BE79A77D-6E82-40E7-8879-451657BD2470}" name="Answer.confidence" dataDxfId="94"/>
-    <tableColumn id="4" xr3:uid="{21C02CF1-E6F8-4239-BC96-BE39B764CBEA}" name="Answer.difficulty" dataDxfId="93"/>
-    <tableColumn id="5" xr3:uid="{C4282863-51A2-429F-A3BC-50D41BBC3125}" name="Answer.explanationSize" dataDxfId="92"/>
-    <tableColumn id="6" xr3:uid="{9256A6DC-68D4-4917-8E93-83FCBD5504DC}" name="Worker.age" dataDxfId="91"/>
-    <tableColumn id="7" xr3:uid="{B5CC5391-D9E0-49B0-95E4-731CDFC8B119}" name="Worker.score" dataDxfId="90"/>
-    <tableColumn id="8" xr3:uid="{F1CEFE01-8A25-4892-8EFF-12BBA59C483B}" name="Worker.yearsOfExperience" dataDxfId="89"/>
-    <tableColumn id="9" xr3:uid="{E0A74493-B88F-40E5-BEC9-8F4B93285734}" name="Code.LOC" dataDxfId="88"/>
-    <tableColumn id="10" xr3:uid="{96BB921C-6A27-4AA9-98A7-349D678C9C71}" name="Code.complexity" dataDxfId="87"/>
+    <tableColumn id="1" xr3:uid="{730CCBB1-AC15-4F76-8658-499BBF9F327F}" name="Spearman Correlations" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{2EF649F7-CBCF-4119-8704-8609DC0A4191}" name="Answer.duration" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{BE79A77D-6E82-40E7-8879-451657BD2470}" name="Answer.confidence" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{21C02CF1-E6F8-4239-BC96-BE39B764CBEA}" name="Answer.difficulty" dataDxfId="73"/>
+    <tableColumn id="5" xr3:uid="{C4282863-51A2-429F-A3BC-50D41BBC3125}" name="Answer.explanationSize" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{9256A6DC-68D4-4917-8E93-83FCBD5504DC}" name="Worker.age" dataDxfId="71"/>
+    <tableColumn id="7" xr3:uid="{B5CC5391-D9E0-49B0-95E4-731CDFC8B119}" name="Worker.score" dataDxfId="70"/>
+    <tableColumn id="8" xr3:uid="{F1CEFE01-8A25-4892-8EFF-12BBA59C483B}" name="Worker.yearsOfExperience" dataDxfId="69"/>
+    <tableColumn id="9" xr3:uid="{E0A74493-B88F-40E5-BEC9-8F4B93285734}" name="Code.LOC" dataDxfId="68"/>
+    <tableColumn id="10" xr3:uid="{96BB921C-6A27-4AA9-98A7-349D678C9C71}" name="Code.complexity" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2329,10 +2563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1796875" defaultRowHeight="14.5"/>
@@ -2350,7 +2584,39 @@
     <col min="11" max="16384" width="18.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="29">
+    <row r="1" spans="1:11">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="29">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2376,13 +2642,16 @@
         <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -2408,13 +2677,16 @@
         <v>0.145769342780113</v>
       </c>
       <c r="I3" s="11">
-        <v>7.1861594915390001E-2</v>
+        <v>-3.6150988191366203E-2</v>
       </c>
       <c r="J3" s="11">
         <v>7.1861594915390001E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="11">
+        <v>7.1861594915390001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -2439,14 +2711,17 @@
       <c r="H4" s="11">
         <v>0.221997395157814</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>12</v>
+      <c r="I4" s="11">
+        <v>5.4549623280763598E-2</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -2472,13 +2747,16 @@
         <v>-0.24901738762855499</v>
       </c>
       <c r="I5" s="11">
+        <v>-8.99812877178192E-2</v>
+      </c>
+      <c r="J5" s="11">
         <v>6.8165458738803905E-2</v>
       </c>
-      <c r="J5" s="11">
+      <c r="K5" s="11">
         <v>3.8963541388511699E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
@@ -2503,14 +2781,17 @@
       <c r="H6" s="11">
         <v>0.22810959815979001</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="11">
+      <c r="I6" s="11">
+        <v>5.8227516710758202E-2</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="11">
         <v>4.1282296180725098E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -2535,14 +2816,17 @@
       <c r="H7" s="11">
         <v>0.55862081050872803</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>12</v>
+      <c r="I7" s="11">
+        <v>-0.32599547505378701</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
@@ -2567,14 +2851,17 @@
       <c r="H8" s="11">
         <v>0.12306752055883401</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="11">
+      <c r="I8" s="11">
+        <v>-6.1543971300125101E-2</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="11">
         <v>-4.0266912430524798E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -2599,450 +2886,516 @@
       <c r="H9" s="12">
         <v>1</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="12">
+        <v>9.8653858003672199E-5</v>
+      </c>
+      <c r="J9" s="11">
         <v>-4.7836016863584498E-2</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="11">
-        <v>7.1861594915390001E-2</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="11">
+        <v>5.4549623280763598E-2</v>
       </c>
       <c r="D10" s="11">
-        <v>6.8165458738803905E-2</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="11">
-        <v>-4.7836016863584498E-2</v>
+        <v>-8.99812877178192E-2</v>
+      </c>
+      <c r="E10" s="11">
+        <v>5.8227516710758202E-2</v>
+      </c>
+      <c r="F10" s="11">
+        <v>-0.32599547505378701</v>
+      </c>
+      <c r="G10" s="11">
+        <v>-6.1543971300125101E-2</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="I10" s="12">
         <v>1</v>
       </c>
       <c r="J10" s="11">
-        <v>0.63391876220703103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>-1.95964202284813E-2</v>
+      </c>
+      <c r="K10" s="12">
+        <v>-8.8582914322614704E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="11">
-        <v>7.5235642492771093E-2</v>
+        <v>7.1861594915390001E-2</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="11">
-        <v>3.8963541388511699E-2</v>
-      </c>
-      <c r="E11" s="11">
-        <v>4.1282296180725098E-2</v>
+        <v>6.8165458738803905E-2</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="11">
-        <v>-4.0266912430524798E-2</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="11">
-        <v>0.63391876220703103</v>
+      <c r="G11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="11">
+        <v>-4.7836016863584498E-2</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="J11" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="5" t="s">
+      <c r="K11" s="11">
+        <v>0.63391876220703103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="11">
+        <v>7.5235642492771093E-2</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="11">
+        <v>3.8963541388511699E-2</v>
+      </c>
+      <c r="E12" s="11">
+        <v>4.1282296180725098E-2</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="11">
+        <v>-4.0266912430524798E-2</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="11">
+        <v>0.63391876220703103</v>
+      </c>
+      <c r="K12" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="29">
+      <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I15" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="K15" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:11">
+      <c r="A16" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C16" s="6">
         <v>2.23961172096665E-6</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D16" s="6">
         <v>3.5306735313156403E-10</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E16" s="6">
         <v>0</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F16" s="6">
         <v>0</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G16" s="6">
         <v>4.2668980684945602E-4</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H16" s="6">
         <v>1.2922996006636799E-13</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I16" s="6"/>
+      <c r="J16" s="6">
         <v>2.7611514861813902E-4</v>
       </c>
-      <c r="J15" s="6">
+      <c r="K16" s="6">
         <v>1.4011664505009201E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="5" t="s">
+    <row r="17" spans="1:11">
+      <c r="A17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B17" s="8">
         <v>2.23961172096665E-6</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D17" s="8">
         <v>0</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E17" s="8">
         <v>4.0153987557189899E-6</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F17" s="8">
         <v>1.46160412084604E-2</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G17" s="8">
         <v>5.3358099624826003E-2</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H17" s="8">
         <v>0</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I17" s="8"/>
+      <c r="J17" s="8">
         <v>5.3194435608916499E-2</v>
       </c>
-      <c r="J16" s="8">
+      <c r="K17" s="8">
         <v>0.23477756000501701</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:11">
+      <c r="A18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B18" s="6">
         <v>3.5306735313156403E-10</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C18" s="6">
         <v>0</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E18" s="6">
         <v>1.4611645227091701E-10</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F18" s="6">
         <v>0.31795557096689597</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G18" s="6">
         <v>1.37773958956977E-5</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H18" s="6">
         <v>0</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I18" s="6"/>
+      <c r="J18" s="6">
         <v>5.6217686439330396E-4</v>
       </c>
-      <c r="J17" s="6">
+      <c r="K18" s="6">
         <v>4.88331220954994E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:11">
+      <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B19" s="8">
         <v>0</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C19" s="8">
         <v>4.0153987557189899E-6</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D19" s="8">
         <v>1.4611645227091701E-10</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F19" s="8">
         <v>1.27575308095373E-8</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G19" s="8">
         <v>7.86154756267088E-5</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H19" s="8">
         <v>0</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I19" s="8"/>
+      <c r="J19" s="8">
         <v>0.92500884385868098</v>
       </c>
-      <c r="J18" s="8">
+      <c r="K19" s="8">
         <v>3.6853600081859998E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:11">
+      <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B20" s="6">
         <v>0</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C20" s="6">
         <v>1.46160412084604E-2</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D20" s="6">
         <v>0.31795557096689597</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E20" s="6">
         <v>1.27575308095373E-8</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G20" s="6">
         <v>9.8348297600794297E-3</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H20" s="6">
         <v>0</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I20" s="6"/>
+      <c r="J20" s="6">
         <v>0.110005151050098</v>
       </c>
-      <c r="J19" s="6">
+      <c r="K20" s="6">
         <v>0.15685758867456601</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:11">
+      <c r="A21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B21" s="8">
         <v>4.2668980684945602E-4</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C21" s="8">
         <v>5.3358099624826003E-2</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D21" s="8">
         <v>1.37773958956977E-5</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E21" s="8">
         <v>7.86154756267088E-5</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F21" s="8">
         <v>9.8348297600794297E-3</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H21" s="8">
         <v>4.2697312352402202E-10</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I21" s="8"/>
+      <c r="J21" s="8">
         <v>0.571172639781235</v>
       </c>
-      <c r="J20" s="8">
+      <c r="K21" s="8">
         <v>4.1750504530216198E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="5" t="s">
+    <row r="22" spans="1:11">
+      <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B22" s="6">
         <v>1.2922996006636799E-13</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C22" s="6">
         <v>0</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D22" s="6">
         <v>0</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E22" s="6">
         <v>0</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F22" s="6">
         <v>0</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G22" s="6">
         <v>4.2697312352402202E-10</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I22" s="6"/>
+      <c r="J22" s="6">
         <v>1.55582857884866E-2</v>
       </c>
-      <c r="J21" s="6">
+      <c r="K22" s="6">
         <v>0.96107509958246196</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:11">
+      <c r="A23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B24" s="8">
         <v>2.7611514861813902E-4</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C24" s="8">
         <v>5.3194435608916499E-2</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D24" s="8">
         <v>5.6217686439330396E-4</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E24" s="8">
         <v>0.92500884385868098</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F24" s="8">
         <v>0.110005151050098</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G24" s="8">
         <v>0.571172639781235</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H24" s="8">
         <v>1.55582857884866E-2</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I24" s="8"/>
+      <c r="J24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J22" s="8">
+      <c r="K24" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="5" t="s">
+    <row r="25" spans="1:11">
+      <c r="A25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B25" s="6">
         <v>1.4011664505009201E-4</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C25" s="6">
         <v>0.23477756000501701</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D25" s="6">
         <v>4.88331220954994E-2</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E25" s="6">
         <v>3.6853600081859998E-2</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F25" s="6">
         <v>0.15685758867456601</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G25" s="6">
         <v>4.1750504530216198E-2</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H25" s="6">
         <v>0.96107509958246196</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I25" s="6"/>
+      <c r="J25" s="6">
         <v>0</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="K25" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
-      <c r="D26" s="10" t="s">
+    <row r="28" spans="1:11">
+      <c r="D28" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
-      <c r="D27" s="10" t="s">
+    <row r="29" spans="1:11">
+      <c r="D29" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="D28" s="10" t="s">
+    <row r="30" spans="1:11">
+      <c r="D30" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
-      <c r="D29" s="10" t="s">
+    <row r="31" spans="1:11">
+      <c r="D31" s="10" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B15:I23">
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="lessThan">
+  <conditionalFormatting sqref="B16:K25">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J15:J23">
-    <cfRule type="cellIs" dxfId="28" priority="7" operator="lessThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:J11">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="between">
+  <conditionalFormatting sqref="B3:K12">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="between">
       <formula>-0.29</formula>
       <formula>-0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="between">
       <formula>0.001</formula>
       <formula>0.29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="between">
       <formula>-0.49</formula>
       <formula>-0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="between">
       <formula>0.3</formula>
       <formula>0.49</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="between">
       <formula>-1</formula>
       <formula>-0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="between">
       <formula>0.5</formula>
       <formula>0.9999999</formula>
     </cfRule>
@@ -3057,10 +3410,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932A3AE4-BA18-48EB-8066-24A92C3920A7}">
-  <dimension ref="B1:K11"/>
+  <dimension ref="B1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3070,11 +3423,13 @@
     <col min="6" max="6" width="10.81640625" customWidth="1"/>
     <col min="8" max="8" width="10.54296875" customWidth="1"/>
     <col min="9" max="9" width="9.7265625" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" customWidth="1"/>
     <col min="11" max="11" width="10.453125" customWidth="1"/>
+    <col min="12" max="12" width="9.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1"/>
-    <row r="2" spans="2:11" ht="44" thickBot="1">
+    <row r="1" spans="2:12" ht="15" thickBot="1"/>
+    <row r="2" spans="2:12" ht="44" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
@@ -3087,336 +3442,427 @@
       <c r="E2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="30" t="s">
+      <c r="J2" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="L2" s="31" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:12">
       <c r="B3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="19">
-        <v>1</v>
-      </c>
-      <c r="D3" s="20">
+      <c r="C3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="19">
         <v>-9.3390814960002899E-2</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="19">
         <v>0.12364736199379001</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="19">
         <v>0.45176514983177202</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="32">
         <v>0.17628009617328599</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="23">
         <v>0.145769342780113</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I3" s="23">
         <v>6.9619752466678606E-2</v>
       </c>
-      <c r="J3" s="33">
+      <c r="J3" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="23">
         <v>7.1861594915390001E-2</v>
       </c>
-      <c r="K3" s="25">
+      <c r="L3" s="23">
         <v>7.1861594915390001E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:12">
       <c r="B4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="21">
         <v>-9.3390814960002899E-2</v>
       </c>
-      <c r="D4" s="23">
-        <v>1</v>
-      </c>
-      <c r="E4" s="24">
+      <c r="D4" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="23">
         <v>-0.57210046052932695</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="23">
         <v>9.1033250093460097E-2</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="32">
         <v>4.8283178359270103E-2</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="23">
         <v>0.221997395157814</v>
       </c>
-      <c r="I4" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11">
+      <c r="I4" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="24">
+        <v>3.8211852312087999E-2</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
       <c r="B5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <v>0.12364736199379001</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>-0.57210046052932695</v>
       </c>
-      <c r="E5" s="23">
-        <v>1</v>
-      </c>
-      <c r="F5" s="25">
+      <c r="E5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="23">
         <v>-0.126304566860199</v>
       </c>
-      <c r="G5" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="24">
+      <c r="G5" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="23">
         <v>-0.24901738762855499</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="23">
         <v>-8.5856214165687603E-2</v>
       </c>
-      <c r="J5" s="33">
+      <c r="J5" s="24">
+        <v>-8.5856214165687603E-2</v>
+      </c>
+      <c r="K5" s="23">
         <v>6.8165458738803905E-2</v>
       </c>
-      <c r="K5" s="25">
+      <c r="L5" s="23">
         <v>3.8963541388511699E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="15" thickBot="1">
+    <row r="6" spans="2:12" ht="15" thickBot="1">
       <c r="B6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="21">
         <v>0.45176514983177202</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="25">
         <v>9.1033250093460097E-2</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="25">
         <v>-0.126304566860199</v>
       </c>
-      <c r="F6" s="29">
-        <v>1</v>
-      </c>
-      <c r="G6" s="33">
+      <c r="F6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="32">
         <v>0.112209625542164</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="23">
         <v>0.22810959815979001</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="23">
         <v>7.8005611896514906E-2</v>
       </c>
-      <c r="J6" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="25">
+      <c r="J6" s="24">
+        <v>7.8005611896514906E-2</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="23">
         <v>4.1282296180725098E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:12">
       <c r="B7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="33">
         <v>0.17628009617328599</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="34">
         <v>4.8283178359270103E-2</v>
       </c>
-      <c r="E7" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="35">
+      <c r="E7" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="34">
         <v>0.112209625542164</v>
       </c>
-      <c r="G7" s="19">
-        <v>1</v>
-      </c>
-      <c r="H7" s="20">
+      <c r="G7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="19">
         <v>0.55862081050872803</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="19">
         <v>5.1044616848230397E-2</v>
       </c>
-      <c r="J7" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11">
+      <c r="J7" s="20">
+        <v>5.1044616848230397E-2</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
       <c r="B8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="21">
         <v>0.145769342780113</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="25">
         <v>0.221997395157814</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="25">
         <v>-0.24901738762855499</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="25">
         <v>0.22810959815979001</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="21">
         <v>0.55862081050872803</v>
       </c>
-      <c r="H8" s="23">
-        <v>1</v>
-      </c>
-      <c r="I8" s="24">
+      <c r="H8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="23">
         <v>0.12306752055883401</v>
       </c>
-      <c r="J8" s="33">
+      <c r="J8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="23">
         <v>-4.7836016863584498E-2</v>
       </c>
-      <c r="K8" s="25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="15" thickBot="1">
+      <c r="L8" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
       <c r="B9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="21">
         <v>6.9619752466678606E-2</v>
       </c>
-      <c r="D9" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="26">
+      <c r="D9" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="25">
         <v>-8.5856214165687603E-2</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="25">
         <v>7.8005611896514906E-2</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="21">
         <v>5.1044616848230397E-2</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="25">
         <v>0.12306752055883401</v>
       </c>
-      <c r="I9" s="23">
-        <v>1</v>
-      </c>
-      <c r="J9" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="25">
+      <c r="I9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="24">
+        <v>-6.1543971300125101E-2</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="24">
         <v>-4.0266912430524798E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:11">
-      <c r="B10" s="13" t="s">
+    <row r="10" spans="2:12" ht="15" thickBot="1">
+      <c r="B10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="42">
+        <v>5.4549623280763598E-2</v>
+      </c>
+      <c r="E10" s="42">
+        <v>-8.99812877178192E-2</v>
+      </c>
+      <c r="F10" s="42">
+        <v>5.8227516710758202E-2</v>
+      </c>
+      <c r="G10" s="41">
+        <v>-0.32599547505378701</v>
+      </c>
+      <c r="H10" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="42">
+        <v>-6.1543971300125101E-2</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C11" s="34">
         <v>7.1861594915390001E-2</v>
       </c>
-      <c r="D10" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="35">
+      <c r="D11" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="34">
         <v>6.8165458738803905E-2</v>
       </c>
-      <c r="F10" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="35">
+      <c r="F11" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="34">
         <v>-4.7836016863584498E-2</v>
       </c>
-      <c r="I10" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="19">
-        <v>1</v>
-      </c>
-      <c r="K10" s="21">
+      <c r="I11" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="20">
         <v>0.63391876220703103</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="15" thickBot="1">
-      <c r="B11" s="15" t="s">
+    <row r="12" spans="2:12" ht="15" thickBot="1">
+      <c r="B12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C12" s="27">
         <v>7.5235642492771093E-2</v>
       </c>
-      <c r="D11" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="28">
+      <c r="D12" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="27">
         <v>3.8963541388511699E-2</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F12" s="27">
         <v>4.1282296180725098E-2</v>
       </c>
-      <c r="G11" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="28">
+      <c r="G12" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="27">
         <v>-4.0266912430524798E-2</v>
       </c>
-      <c r="J11" s="27">
+      <c r="J12" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="26">
         <v>0.63391876220703103</v>
       </c>
-      <c r="K11" s="29">
-        <v>1</v>
+      <c r="L12" s="28" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3 C6:F6 C5:E5 C4:D4 I9 J11:K11 J10 C10:I11 C8:H9 C7:G7">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="between">
+  <conditionalFormatting sqref="C3 C6:F6 C5:E5 C4:D4 I9 K11 C8:H9 C7:G7 J10 K12:L12 C10:I12">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="between">
       <formula>-0.29</formula>
       <formula>-0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="14" operator="between">
       <formula>0.001</formula>
       <formula>0.29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="15" operator="between">
       <formula>-0.49</formula>
       <formula>-0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="16" operator="between">
       <formula>0.3</formula>
       <formula>0.49</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="17" operator="between">
       <formula>-1</formula>
       <formula>-0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="18" operator="between">
+      <formula>0.5</formula>
+      <formula>0.9999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11:J12">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="between">
+      <formula>-0.29</formula>
+      <formula>-0.001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="between">
+      <formula>0.001</formula>
+      <formula>0.29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="between">
+      <formula>-0.49</formula>
+      <formula>-0.3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="between">
+      <formula>0.3</formula>
+      <formula>0.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="between">
+      <formula>-1</formula>
+      <formula>-0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="between">
       <formula>0.5</formula>
       <formula>0.9999999</formula>
     </cfRule>
@@ -4086,12 +4532,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>$B$15&lt;0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:I23">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4101,4 +4547,236 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA20E1B-DD68-44BD-9EFD-0E020BB54BBD}">
+  <dimension ref="B2:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="25.90625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="15" thickBot="1"/>
+    <row r="3" spans="2:5" ht="29.5" thickBot="1">
+      <c r="B3" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="40">
+        <v>-2.4937109999999998E-2</v>
+      </c>
+      <c r="E4" s="51">
+        <v>0.1227876</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="63">
+        <v>1</v>
+      </c>
+      <c r="D5" s="25">
+        <v>1</v>
+      </c>
+      <c r="E5" s="39">
+        <v>2.7777779999999998E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="50">
+        <v>-0.4</v>
+      </c>
+      <c r="E6" s="52">
+        <v>0.48333330000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15" thickBot="1">
+      <c r="B7" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="66">
+        <v>-0.61235799999999996</v>
+      </c>
+      <c r="D7" s="27">
+        <v>-0.61235799999999996</v>
+      </c>
+      <c r="E7" s="53">
+        <v>9.8505169999999996E-75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="67">
+        <v>-0.63130410000000003</v>
+      </c>
+      <c r="D8" s="54">
+        <v>-0.63130410000000003</v>
+      </c>
+      <c r="E8" s="55">
+        <v>1.7426419999999999E-9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="63">
+        <v>-0.30001080000000002</v>
+      </c>
+      <c r="D9" s="25">
+        <v>-0.30001080000000002</v>
+      </c>
+      <c r="E9" s="39">
+        <v>1.185164E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="E10" s="39">
+        <v>0.81666669999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15" thickBot="1">
+      <c r="B11" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="25">
+        <v>1</v>
+      </c>
+      <c r="E11" s="57">
+        <v>0.3333333</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="68">
+        <v>-0.53436669999999997</v>
+      </c>
+      <c r="D12" s="34">
+        <v>-0.53436669999999997</v>
+      </c>
+      <c r="E12" s="58">
+        <v>1.6141429999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15" thickBot="1">
+      <c r="B13" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="69">
+        <v>-0.90476190000000001</v>
+      </c>
+      <c r="D13" s="56">
+        <v>-0.90476190000000001</v>
+      </c>
+      <c r="E13" s="59">
+        <v>2.7777779999999998E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D4:D13">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="between">
+      <formula>-0.29</formula>
+      <formula>-0.001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="between">
+      <formula>0.001</formula>
+      <formula>0.29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="between">
+      <formula>-0.49</formula>
+      <formula>-0.3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="17" operator="between">
+      <formula>0.3</formula>
+      <formula>0.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="18" operator="between">
+      <formula>-1</formula>
+      <formula>-0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="19" stopIfTrue="1" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E13">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C13">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="between">
+      <formula>-0.29</formula>
+      <formula>-0.001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+      <formula>0.001</formula>
+      <formula>0.29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
+      <formula>-0.49</formula>
+      <formula>-0.3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
+      <formula>0.3</formula>
+      <formula>0.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="between">
+      <formula>-1</formula>
+      <formula>-0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" stopIfTrue="1" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>